<commit_message>
school admin dashboard update
</commit_message>
<xml_diff>
--- a/Backend/staticfiles/st_augustines_senior_high_school/staff/Schooladministrator/MATHEMATICS.xlsx
+++ b/Backend/staticfiles/st_augustines_senior_high_school/staff/Schooladministrator/MATHEMATICS.xlsx
@@ -77,7 +77,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -109,12 +109,6 @@
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -497,17 +491,17 @@
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18.28515625" customWidth="1" min="1" max="1"/>
-    <col width="21.140625" customWidth="1" min="2" max="2"/>
-    <col width="17.7109375" customWidth="1" style="1" min="3" max="3"/>
-    <col width="20.7109375" customWidth="1" style="1" min="4" max="4"/>
-    <col width="24" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
-    <col width="34.28515625" customWidth="1" style="7" min="6" max="6"/>
+    <col width="38.5703125" customWidth="1" min="1" max="1"/>
+    <col width="48.42578125" customWidth="1" min="2" max="2"/>
+    <col width="19.7109375" customWidth="1" style="1" min="3" max="3"/>
+    <col width="12.42578125" customWidth="1" style="1" min="4" max="4"/>
+    <col width="24.28515625" customWidth="1" style="2" min="5" max="5"/>
+    <col width="43" customWidth="1" style="7" min="6" max="6"/>
     <col width="10" bestFit="1" customWidth="1" min="7" max="7"/>
     <col width="12.7109375" bestFit="1" customWidth="1" min="8" max="8"/>
     <col width="10.5703125" bestFit="1" customWidth="1" min="11" max="11"/>
@@ -531,22 +525,22 @@
       </c>
     </row>
     <row r="3" ht="22.5" customHeight="1">
-      <c r="A3" s="11" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>FIRST NAME</t>
         </is>
       </c>
-      <c r="B3" s="11" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>LAST NAME</t>
         </is>
       </c>
-      <c r="C3" s="11" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>STAFF ID</t>
         </is>
       </c>
-      <c r="D3" s="11" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>GENDER</t>
         </is>
@@ -556,29 +550,29 @@
           <t>DATE OF BIRTH</t>
         </is>
       </c>
-      <c r="F3" s="11" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>SUBJECTS(S)</t>
         </is>
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
-      <c r="A4" s="12" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Eg. JUSTICE</t>
         </is>
       </c>
-      <c r="B4" s="12" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr">
         <is>
           <t>Eg. NYAME</t>
         </is>
       </c>
-      <c r="C4" s="12" t="inlineStr">
+      <c r="C4" s="4" t="inlineStr">
         <is>
           <t>Eg. 20719127</t>
         </is>
       </c>
-      <c r="D4" s="12" t="inlineStr">
+      <c r="D4" s="4" t="inlineStr">
         <is>
           <t>MALE</t>
         </is>
@@ -588,7 +582,7 @@
           <t>1999-09-26 OR 26/09/1999</t>
         </is>
       </c>
-      <c r="F4" s="12" t="inlineStr">
+      <c r="F4" s="4" t="inlineStr">
         <is>
           <t>Eg. BIOLOGY OR PHYSICS,CHEMISTRY</t>
         </is>
@@ -598,7 +592,11 @@
       <c r="A5" s="7" t="n"/>
       <c r="B5" s="7" t="n"/>
       <c r="C5" s="8" t="n"/>
-      <c r="D5" s="8" t="n"/>
+      <c r="D5" s="8" t="inlineStr">
+        <is>
+          <t>MALE</t>
+        </is>
+      </c>
       <c r="E5" s="9" t="n"/>
     </row>
     <row r="6">

</xml_diff>